<commit_message>
latest commit w updated cardinal directions
</commit_message>
<xml_diff>
--- a/dist/result.xlsx
+++ b/dist/result.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://powereng0-my.sharepoint.com/personal/ashim_dhakal_powereng_com/Documents/Desktop/pythonDB/dist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_B00C2D506BB74EF824D2B8782CD8C01686C026BE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4ABFB813-3EC0-40CF-9A4B-861E96F9571A}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_B00C2D506BB74EF824D2B8782CD8C01686C026BE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02B7F1EE-CE77-4B41-A492-5B9C8388D298}"/>
   <bookViews>
-    <workbookView xWindow="-17280" yWindow="1365" windowWidth="17280" windowHeight="10050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Report" sheetId="1" r:id="rId1"/>
-    <sheet name="Primary Stringing Data" sheetId="2" r:id="rId2"/>
-    <sheet name="Neutral Span Stringing Data" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Primary Stringing Data" sheetId="2" r:id="rId3"/>
+    <sheet name="Neutral Span Stringing Data" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2950" uniqueCount="1154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3139" uniqueCount="1157">
   <si>
     <t>sequence</t>
   </si>
@@ -3484,6 +3485,15 @@
   </si>
   <si>
     <t>4200.70</t>
+  </si>
+  <si>
+    <t>p1 lat</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>p1 long</t>
   </si>
 </sst>
 </file>
@@ -3851,8 +3861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection sqref="A1:R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12982,6 +12992,748 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7353EA6-ED35-4EB9-9D46-1CE956C9A6AB}">
+  <dimension ref="A1:R17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection sqref="A1:R8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="24.109375" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" customWidth="1"/>
+    <col min="10" max="10" width="50.88671875" customWidth="1"/>
+    <col min="13" max="13" width="18.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1155</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>1154</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>1156</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>1155</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>1154</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>1154</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>1156</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>1154</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
@@ -14153,7 +14905,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D56"/>
   <sheetViews>

</xml_diff>